<commit_message>
updated last edited time
</commit_message>
<xml_diff>
--- a/Design Data/Sample Data/Excel Files/last edited time.xlsx
+++ b/Design Data/Sample Data/Excel Files/last edited time.xlsx
@@ -1,12 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S538408\Documents\GDP\gdp_health_app\Design Data\Sample Data\Excel Files\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F0C88FA-9409-4FF8-ACE0-49A48BAD1C4D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -526,25 +535,24 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
-    <numFmt numFmtId="165" formatCode="m/d/yy h:mm am/pm"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="m/d/yy\ h:mm\ AM/PM"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
       <b/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
@@ -554,7 +562,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -564,47 +572,52 @@
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="7">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -794,20 +807,28 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:F178"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="18.36328125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -825,3186 +846,3186 @@
       </c>
       <c r="F1" s="3"/>
     </row>
-    <row r="2">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="4">
-        <v>222.0</v>
+        <v>222</v>
       </c>
       <c r="B2" s="4">
-        <v>124.0</v>
+        <v>124</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D2" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E2" s="6">
         <v>44067.15625</v>
       </c>
       <c r="F2" s="3"/>
     </row>
-    <row r="3">
+    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="4">
-        <v>223.0</v>
+        <v>223</v>
       </c>
       <c r="B3" s="4">
-        <v>125.0</v>
+        <v>125</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D3" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E3" s="6">
         <v>44067.416666666664</v>
       </c>
       <c r="F3" s="3"/>
     </row>
-    <row r="4">
+    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="4">
-        <v>224.0</v>
+        <v>224</v>
       </c>
       <c r="B4" s="4">
-        <v>126.0</v>
+        <v>126</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>7</v>
       </c>
       <c r="D4" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E4" s="6">
         <v>44067.4375</v>
       </c>
       <c r="F4" s="3"/>
     </row>
-    <row r="5">
+    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="4">
-        <v>225.0</v>
+        <v>225</v>
       </c>
       <c r="B5" s="4">
-        <v>127.0</v>
+        <v>127</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D5" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E5" s="6">
         <v>44067.375</v>
       </c>
       <c r="F5" s="3"/>
     </row>
-    <row r="6">
+    <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="4">
-        <v>226.0</v>
+        <v>226</v>
       </c>
       <c r="B6" s="4">
-        <v>128.0</v>
+        <v>128</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D6" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E6" s="6">
         <v>44066.75</v>
       </c>
       <c r="F6" s="3"/>
     </row>
-    <row r="7">
+    <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="4">
-        <v>227.0</v>
+        <v>227</v>
       </c>
       <c r="B7" s="4">
-        <v>129.0</v>
+        <v>129</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D7" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E7" s="6">
         <v>44066.833333333336</v>
       </c>
       <c r="F7" s="3"/>
     </row>
-    <row r="8">
+    <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="4">
-        <v>228.0</v>
+        <v>228</v>
       </c>
       <c r="B8" s="4">
-        <v>130.0</v>
+        <v>130</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D8" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E8" s="6">
         <v>44067.395833333336</v>
       </c>
       <c r="F8" s="3"/>
     </row>
-    <row r="9">
+    <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="4">
-        <v>229.0</v>
+        <v>229</v>
       </c>
       <c r="B9" s="4">
-        <v>131.0</v>
+        <v>131</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D9" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E9" s="6">
         <v>44067.15625</v>
       </c>
       <c r="F9" s="3"/>
     </row>
-    <row r="10">
+    <row r="10" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="4">
-        <v>230.0</v>
+        <v>230</v>
       </c>
       <c r="B10" s="4">
-        <v>132.0</v>
+        <v>132</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>12</v>
       </c>
       <c r="D10" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E10" s="6">
         <v>44067.416666666664</v>
       </c>
       <c r="F10" s="3"/>
     </row>
-    <row r="11">
+    <row r="11" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="4">
-        <v>231.0</v>
+        <v>231</v>
       </c>
       <c r="B11" s="4">
-        <v>133.0</v>
+        <v>133</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D11" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E11" s="6">
         <v>44067.4375</v>
       </c>
       <c r="F11" s="3"/>
     </row>
-    <row r="12">
+    <row r="12" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="4">
-        <v>232.0</v>
+        <v>232</v>
       </c>
       <c r="B12" s="4">
-        <v>134.0</v>
+        <v>134</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>14</v>
       </c>
       <c r="D12" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E12" s="6">
         <v>44067.375</v>
       </c>
       <c r="F12" s="3"/>
     </row>
-    <row r="13">
+    <row r="13" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="4">
-        <v>233.0</v>
+        <v>233</v>
       </c>
       <c r="B13" s="4">
-        <v>135.0</v>
+        <v>135</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>15</v>
       </c>
       <c r="D13" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E13" s="6">
         <v>44066.75</v>
       </c>
       <c r="F13" s="3"/>
     </row>
-    <row r="14">
+    <row r="14" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="4">
-        <v>234.0</v>
+        <v>234</v>
       </c>
       <c r="B14" s="4">
-        <v>136.0</v>
+        <v>136</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>16</v>
       </c>
       <c r="D14" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E14" s="6">
         <v>44066.833333333336</v>
       </c>
       <c r="F14" s="3"/>
     </row>
-    <row r="15">
+    <row r="15" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="4">
-        <v>235.0</v>
+        <v>235</v>
       </c>
       <c r="B15" s="4">
-        <v>137.0</v>
+        <v>137</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>16</v>
       </c>
       <c r="D15" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E15" s="6">
         <v>44067.395833333336</v>
       </c>
       <c r="F15" s="3"/>
     </row>
-    <row r="16">
+    <row r="16" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="4">
-        <v>236.0</v>
+        <v>236</v>
       </c>
       <c r="B16" s="4">
-        <v>138.0</v>
+        <v>138</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>17</v>
       </c>
       <c r="D16" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E16" s="6">
         <v>44067.15625</v>
       </c>
       <c r="F16" s="3"/>
     </row>
-    <row r="17">
+    <row r="17" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="4">
-        <v>237.0</v>
+        <v>237</v>
       </c>
       <c r="B17" s="4">
-        <v>139.0</v>
+        <v>139</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>18</v>
       </c>
       <c r="D17" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E17" s="6">
         <v>44067.416666666664</v>
       </c>
       <c r="F17" s="3"/>
     </row>
-    <row r="18">
+    <row r="18" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="4">
-        <v>238.0</v>
+        <v>238</v>
       </c>
       <c r="B18" s="4">
-        <v>140.0</v>
+        <v>140</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>19</v>
       </c>
       <c r="D18" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E18" s="6">
         <v>44067.4375</v>
       </c>
       <c r="F18" s="3"/>
     </row>
-    <row r="19">
+    <row r="19" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="4">
-        <v>239.0</v>
+        <v>239</v>
       </c>
       <c r="B19" s="4">
-        <v>141.0</v>
+        <v>141</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>20</v>
       </c>
       <c r="D19" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E19" s="6">
         <v>44067.375</v>
       </c>
       <c r="F19" s="3"/>
     </row>
-    <row r="20">
+    <row r="20" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="4">
-        <v>240.0</v>
+        <v>240</v>
       </c>
       <c r="B20" s="4">
-        <v>142.0</v>
+        <v>142</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>21</v>
       </c>
       <c r="D20" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E20" s="6">
         <v>44066.75</v>
       </c>
       <c r="F20" s="3"/>
     </row>
-    <row r="21">
+    <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="4">
-        <v>241.0</v>
+        <v>241</v>
       </c>
       <c r="B21" s="4">
-        <v>143.0</v>
+        <v>143</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>21</v>
       </c>
       <c r="D21" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E21" s="6">
         <v>44066.833333333336</v>
       </c>
       <c r="F21" s="3"/>
     </row>
-    <row r="22">
+    <row r="22" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="4">
-        <v>242.0</v>
+        <v>242</v>
       </c>
       <c r="B22" s="4">
-        <v>144.0</v>
+        <v>144</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>21</v>
       </c>
       <c r="D22" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E22" s="6">
         <v>44067.395833333336</v>
       </c>
       <c r="F22" s="3"/>
     </row>
-    <row r="23">
+    <row r="23" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="4">
-        <v>243.0</v>
+        <v>243</v>
       </c>
       <c r="B23" s="4">
-        <v>145.0</v>
+        <v>145</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>22</v>
       </c>
       <c r="D23" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E23" s="6">
         <v>44067.15625</v>
       </c>
       <c r="F23" s="3"/>
     </row>
-    <row r="24">
+    <row r="24" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="4">
-        <v>244.0</v>
+        <v>244</v>
       </c>
       <c r="B24" s="4">
-        <v>146.0</v>
+        <v>146</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>23</v>
       </c>
       <c r="D24" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E24" s="6">
         <v>44067.416666666664</v>
       </c>
       <c r="F24" s="3"/>
     </row>
-    <row r="25">
+    <row r="25" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="4">
-        <v>245.0</v>
+        <v>245</v>
       </c>
       <c r="B25" s="4">
-        <v>147.0</v>
+        <v>147</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>24</v>
       </c>
       <c r="D25" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E25" s="6">
         <v>44067.4375</v>
       </c>
       <c r="F25" s="3"/>
     </row>
-    <row r="26">
+    <row r="26" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="4">
-        <v>246.0</v>
+        <v>246</v>
       </c>
       <c r="B26" s="4">
-        <v>148.0</v>
+        <v>148</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>25</v>
       </c>
       <c r="D26" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E26" s="6">
         <v>44067.375</v>
       </c>
       <c r="F26" s="3"/>
     </row>
-    <row r="27">
+    <row r="27" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="4">
-        <v>247.0</v>
+        <v>247</v>
       </c>
       <c r="B27" s="4">
-        <v>149.0</v>
+        <v>149</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>26</v>
       </c>
       <c r="D27" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E27" s="6">
         <v>44066.75</v>
       </c>
       <c r="F27" s="3"/>
     </row>
-    <row r="28">
+    <row r="28" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="4">
-        <v>248.0</v>
+        <v>248</v>
       </c>
       <c r="B28" s="4">
-        <v>150.0</v>
+        <v>150</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>27</v>
       </c>
       <c r="D28" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E28" s="6">
         <v>44066.833333333336</v>
       </c>
       <c r="F28" s="3"/>
     </row>
-    <row r="29">
+    <row r="29" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A29" s="4">
-        <v>249.0</v>
+        <v>249</v>
       </c>
       <c r="B29" s="4">
-        <v>151.0</v>
+        <v>151</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>28</v>
       </c>
       <c r="D29" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E29" s="6">
         <v>44067.395833333336</v>
       </c>
       <c r="F29" s="3"/>
     </row>
-    <row r="30">
+    <row r="30" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A30" s="4">
-        <v>250.0</v>
+        <v>250</v>
       </c>
       <c r="B30" s="4">
-        <v>152.0</v>
+        <v>152</v>
       </c>
       <c r="C30" s="4" t="s">
         <v>29</v>
       </c>
       <c r="D30" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E30" s="6">
         <v>44067.15625</v>
       </c>
       <c r="F30" s="3"/>
     </row>
-    <row r="31">
+    <row r="31" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A31" s="4">
-        <v>251.0</v>
+        <v>251</v>
       </c>
       <c r="B31" s="4">
-        <v>153.0</v>
+        <v>153</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>30</v>
       </c>
       <c r="D31" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E31" s="6">
         <v>44067.416666666664</v>
       </c>
       <c r="F31" s="3"/>
     </row>
-    <row r="32">
+    <row r="32" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A32" s="4">
-        <v>252.0</v>
+        <v>252</v>
       </c>
       <c r="B32" s="4">
-        <v>154.0</v>
+        <v>154</v>
       </c>
       <c r="C32" s="4" t="s">
         <v>31</v>
       </c>
       <c r="D32" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E32" s="6">
         <v>44067.4375</v>
       </c>
       <c r="F32" s="3"/>
     </row>
-    <row r="33">
+    <row r="33" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A33" s="4">
-        <v>253.0</v>
+        <v>253</v>
       </c>
       <c r="B33" s="4">
-        <v>155.0</v>
+        <v>155</v>
       </c>
       <c r="C33" s="4" t="s">
         <v>32</v>
       </c>
       <c r="D33" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E33" s="6">
         <v>44067.375</v>
       </c>
       <c r="F33" s="3"/>
     </row>
-    <row r="34">
+    <row r="34" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A34" s="4">
-        <v>254.0</v>
+        <v>254</v>
       </c>
       <c r="B34" s="4">
-        <v>156.0</v>
+        <v>156</v>
       </c>
       <c r="C34" s="4" t="s">
         <v>33</v>
       </c>
       <c r="D34" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E34" s="6">
         <v>44066.75</v>
       </c>
       <c r="F34" s="3"/>
     </row>
-    <row r="35">
+    <row r="35" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A35" s="4">
-        <v>255.0</v>
+        <v>255</v>
       </c>
       <c r="B35" s="4">
-        <v>157.0</v>
+        <v>157</v>
       </c>
       <c r="C35" s="4" t="s">
         <v>34</v>
       </c>
       <c r="D35" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E35" s="6">
         <v>44066.833333333336</v>
       </c>
       <c r="F35" s="3"/>
     </row>
-    <row r="36">
+    <row r="36" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A36" s="4">
-        <v>256.0</v>
+        <v>256</v>
       </c>
       <c r="B36" s="4">
-        <v>158.0</v>
+        <v>158</v>
       </c>
       <c r="C36" s="4" t="s">
         <v>35</v>
       </c>
       <c r="D36" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E36" s="6">
         <v>44067.395833333336</v>
       </c>
       <c r="F36" s="3"/>
     </row>
-    <row r="37">
+    <row r="37" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A37" s="4">
-        <v>257.0</v>
+        <v>257</v>
       </c>
       <c r="B37" s="4">
-        <v>159.0</v>
+        <v>159</v>
       </c>
       <c r="C37" s="4" t="s">
         <v>36</v>
       </c>
       <c r="D37" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E37" s="6">
         <v>44067.15625</v>
       </c>
       <c r="F37" s="3"/>
     </row>
-    <row r="38">
+    <row r="38" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A38" s="4">
-        <v>258.0</v>
+        <v>258</v>
       </c>
       <c r="B38" s="4">
-        <v>160.0</v>
+        <v>160</v>
       </c>
       <c r="C38" s="4" t="s">
         <v>37</v>
       </c>
       <c r="D38" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E38" s="6">
         <v>44067.416666666664</v>
       </c>
       <c r="F38" s="3"/>
     </row>
-    <row r="39">
+    <row r="39" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A39" s="4">
-        <v>259.0</v>
+        <v>259</v>
       </c>
       <c r="B39" s="4">
-        <v>161.0</v>
+        <v>161</v>
       </c>
       <c r="C39" s="4" t="s">
         <v>38</v>
       </c>
       <c r="D39" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E39" s="6">
         <v>44067.4375</v>
       </c>
       <c r="F39" s="3"/>
     </row>
-    <row r="40">
+    <row r="40" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A40" s="4">
-        <v>260.0</v>
+        <v>260</v>
       </c>
       <c r="B40" s="4">
-        <v>162.0</v>
+        <v>162</v>
       </c>
       <c r="C40" s="4" t="s">
         <v>39</v>
       </c>
       <c r="D40" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E40" s="6">
         <v>44067.375</v>
       </c>
       <c r="F40" s="3"/>
     </row>
-    <row r="41">
+    <row r="41" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A41" s="4">
-        <v>261.0</v>
+        <v>261</v>
       </c>
       <c r="B41" s="4">
-        <v>163.0</v>
+        <v>163</v>
       </c>
       <c r="C41" s="4" t="s">
         <v>40</v>
       </c>
       <c r="D41" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E41" s="6">
         <v>44066.75</v>
       </c>
       <c r="F41" s="3"/>
     </row>
-    <row r="42">
+    <row r="42" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A42" s="4">
-        <v>262.0</v>
+        <v>262</v>
       </c>
       <c r="B42" s="4">
-        <v>164.0</v>
+        <v>164</v>
       </c>
       <c r="C42" s="4" t="s">
         <v>41</v>
       </c>
       <c r="D42" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E42" s="6">
         <v>44066.833333333336</v>
       </c>
       <c r="F42" s="3"/>
     </row>
-    <row r="43">
+    <row r="43" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A43" s="4">
-        <v>263.0</v>
+        <v>263</v>
       </c>
       <c r="B43" s="4">
-        <v>165.0</v>
+        <v>165</v>
       </c>
       <c r="C43" s="4" t="s">
         <v>42</v>
       </c>
       <c r="D43" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E43" s="6">
         <v>44067.395833333336</v>
       </c>
       <c r="F43" s="3"/>
     </row>
-    <row r="44">
+    <row r="44" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A44" s="4">
-        <v>264.0</v>
+        <v>264</v>
       </c>
       <c r="B44" s="4">
-        <v>166.0</v>
+        <v>166</v>
       </c>
       <c r="C44" s="4" t="s">
         <v>43</v>
       </c>
       <c r="D44" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E44" s="6">
         <v>44067.15625</v>
       </c>
       <c r="F44" s="3"/>
     </row>
-    <row r="45">
+    <row r="45" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A45" s="4">
-        <v>265.0</v>
+        <v>265</v>
       </c>
       <c r="B45" s="4">
-        <v>167.0</v>
+        <v>167</v>
       </c>
       <c r="C45" s="4" t="s">
         <v>44</v>
       </c>
       <c r="D45" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E45" s="6">
         <v>44067.416666666664</v>
       </c>
       <c r="F45" s="3"/>
     </row>
-    <row r="46">
+    <row r="46" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A46" s="4">
-        <v>266.0</v>
+        <v>266</v>
       </c>
       <c r="B46" s="4">
-        <v>168.0</v>
+        <v>168</v>
       </c>
       <c r="C46" s="4" t="s">
         <v>45</v>
       </c>
       <c r="D46" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E46" s="6">
         <v>44067.4375</v>
       </c>
       <c r="F46" s="3"/>
     </row>
-    <row r="47">
+    <row r="47" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A47" s="4">
-        <v>267.0</v>
+        <v>267</v>
       </c>
       <c r="B47" s="4">
-        <v>169.0</v>
+        <v>169</v>
       </c>
       <c r="C47" s="4" t="s">
         <v>46</v>
       </c>
       <c r="D47" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E47" s="6">
         <v>44067.375</v>
       </c>
       <c r="F47" s="3"/>
     </row>
-    <row r="48">
+    <row r="48" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A48" s="4">
-        <v>268.0</v>
+        <v>268</v>
       </c>
       <c r="B48" s="4">
-        <v>170.0</v>
+        <v>170</v>
       </c>
       <c r="C48" s="4" t="s">
         <v>47</v>
       </c>
       <c r="D48" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E48" s="6">
         <v>44066.75</v>
       </c>
       <c r="F48" s="3"/>
     </row>
-    <row r="49">
+    <row r="49" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A49" s="4">
-        <v>269.0</v>
+        <v>269</v>
       </c>
       <c r="B49" s="4">
-        <v>171.0</v>
+        <v>171</v>
       </c>
       <c r="C49" s="4" t="s">
         <v>48</v>
       </c>
       <c r="D49" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E49" s="6">
         <v>44066.833333333336</v>
       </c>
       <c r="F49" s="3"/>
     </row>
-    <row r="50">
+    <row r="50" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A50" s="4">
-        <v>270.0</v>
+        <v>270</v>
       </c>
       <c r="B50" s="4">
-        <v>172.0</v>
+        <v>172</v>
       </c>
       <c r="C50" s="4" t="s">
         <v>49</v>
       </c>
       <c r="D50" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E50" s="6">
         <v>44067.395833333336</v>
       </c>
       <c r="F50" s="3"/>
     </row>
-    <row r="51">
+    <row r="51" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A51" s="4">
-        <v>271.0</v>
+        <v>271</v>
       </c>
       <c r="B51" s="4">
-        <v>173.0</v>
+        <v>173</v>
       </c>
       <c r="C51" s="4" t="s">
         <v>50</v>
       </c>
       <c r="D51" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E51" s="6">
         <v>44067.15625</v>
       </c>
       <c r="F51" s="3"/>
     </row>
-    <row r="52">
+    <row r="52" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A52" s="4">
-        <v>272.0</v>
+        <v>272</v>
       </c>
       <c r="B52" s="4">
-        <v>174.0</v>
+        <v>174</v>
       </c>
       <c r="C52" s="4" t="s">
         <v>51</v>
       </c>
       <c r="D52" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E52" s="6">
         <v>44067.416666666664</v>
       </c>
       <c r="F52" s="3"/>
     </row>
-    <row r="53">
+    <row r="53" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A53" s="4">
-        <v>273.0</v>
+        <v>273</v>
       </c>
       <c r="B53" s="4">
-        <v>175.0</v>
+        <v>175</v>
       </c>
       <c r="C53" s="4" t="s">
         <v>52</v>
       </c>
       <c r="D53" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E53" s="6">
         <v>44067.4375</v>
       </c>
       <c r="F53" s="3"/>
     </row>
-    <row r="54">
+    <row r="54" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A54" s="4">
-        <v>274.0</v>
+        <v>274</v>
       </c>
       <c r="B54" s="4">
-        <v>176.0</v>
+        <v>176</v>
       </c>
       <c r="C54" s="4" t="s">
         <v>53</v>
       </c>
       <c r="D54" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E54" s="6">
         <v>44067.375</v>
       </c>
       <c r="F54" s="3"/>
     </row>
-    <row r="55">
+    <row r="55" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A55" s="4">
-        <v>275.0</v>
+        <v>275</v>
       </c>
       <c r="B55" s="4">
-        <v>177.0</v>
+        <v>177</v>
       </c>
       <c r="C55" s="4" t="s">
         <v>54</v>
       </c>
       <c r="D55" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E55" s="6">
         <v>44066.75</v>
       </c>
       <c r="F55" s="3"/>
     </row>
-    <row r="56">
+    <row r="56" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A56" s="4">
-        <v>276.0</v>
+        <v>276</v>
       </c>
       <c r="B56" s="4">
-        <v>178.0</v>
+        <v>178</v>
       </c>
       <c r="C56" s="4" t="s">
         <v>55</v>
       </c>
       <c r="D56" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E56" s="6">
         <v>44066.833333333336</v>
       </c>
       <c r="F56" s="3"/>
     </row>
-    <row r="57">
+    <row r="57" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A57" s="4">
-        <v>277.0</v>
+        <v>277</v>
       </c>
       <c r="B57" s="4">
-        <v>179.0</v>
+        <v>179</v>
       </c>
       <c r="C57" s="4" t="s">
         <v>56</v>
       </c>
       <c r="D57" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E57" s="6">
         <v>44067.395833333336</v>
       </c>
       <c r="F57" s="3"/>
     </row>
-    <row r="58">
+    <row r="58" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A58" s="4">
-        <v>278.0</v>
+        <v>278</v>
       </c>
       <c r="B58" s="4">
-        <v>180.0</v>
+        <v>180</v>
       </c>
       <c r="C58" s="4" t="s">
         <v>57</v>
       </c>
       <c r="D58" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E58" s="6">
         <v>44067.15625</v>
       </c>
       <c r="F58" s="3"/>
     </row>
-    <row r="59">
+    <row r="59" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A59" s="4">
-        <v>279.0</v>
+        <v>279</v>
       </c>
       <c r="B59" s="4">
-        <v>181.0</v>
+        <v>181</v>
       </c>
       <c r="C59" s="4" t="s">
         <v>58</v>
       </c>
       <c r="D59" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E59" s="6">
         <v>44067.416666666664</v>
       </c>
       <c r="F59" s="3"/>
     </row>
-    <row r="60">
+    <row r="60" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A60" s="4">
-        <v>280.0</v>
+        <v>280</v>
       </c>
       <c r="B60" s="4">
-        <v>182.0</v>
+        <v>182</v>
       </c>
       <c r="C60" s="4" t="s">
         <v>59</v>
       </c>
       <c r="D60" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E60" s="6">
         <v>44067.4375</v>
       </c>
       <c r="F60" s="3"/>
     </row>
-    <row r="61">
+    <row r="61" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A61" s="4">
-        <v>281.0</v>
+        <v>281</v>
       </c>
       <c r="B61" s="4">
-        <v>183.0</v>
+        <v>183</v>
       </c>
       <c r="C61" s="4" t="s">
         <v>59</v>
       </c>
       <c r="D61" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E61" s="6">
         <v>44067.375</v>
       </c>
       <c r="F61" s="3"/>
     </row>
-    <row r="62">
+    <row r="62" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A62" s="4">
-        <v>282.0</v>
+        <v>282</v>
       </c>
       <c r="B62" s="4">
-        <v>184.0</v>
+        <v>184</v>
       </c>
       <c r="C62" s="4" t="s">
         <v>60</v>
       </c>
       <c r="D62" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E62" s="6">
         <v>44066.75</v>
       </c>
       <c r="F62" s="3"/>
     </row>
-    <row r="63">
+    <row r="63" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A63" s="4">
-        <v>283.0</v>
+        <v>283</v>
       </c>
       <c r="B63" s="4">
-        <v>185.0</v>
+        <v>185</v>
       </c>
       <c r="C63" s="4" t="s">
         <v>61</v>
       </c>
       <c r="D63" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E63" s="6">
         <v>44066.833333333336</v>
       </c>
       <c r="F63" s="3"/>
     </row>
-    <row r="64">
+    <row r="64" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A64" s="4">
-        <v>284.0</v>
+        <v>284</v>
       </c>
       <c r="B64" s="4">
-        <v>186.0</v>
+        <v>186</v>
       </c>
       <c r="C64" s="4" t="s">
         <v>62</v>
       </c>
       <c r="D64" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E64" s="6">
         <v>44067.395833333336</v>
       </c>
       <c r="F64" s="3"/>
     </row>
-    <row r="65">
+    <row r="65" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A65" s="4">
-        <v>285.0</v>
+        <v>285</v>
       </c>
       <c r="B65" s="4">
-        <v>187.0</v>
+        <v>187</v>
       </c>
       <c r="C65" s="4" t="s">
         <v>63</v>
       </c>
       <c r="D65" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E65" s="6">
         <v>44067.15625</v>
       </c>
       <c r="F65" s="3"/>
     </row>
-    <row r="66">
+    <row r="66" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A66" s="4">
-        <v>286.0</v>
+        <v>286</v>
       </c>
       <c r="B66" s="4">
-        <v>188.0</v>
+        <v>188</v>
       </c>
       <c r="C66" s="4" t="s">
         <v>64</v>
       </c>
       <c r="D66" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E66" s="6">
         <v>44067.416666666664</v>
       </c>
       <c r="F66" s="3"/>
     </row>
-    <row r="67">
+    <row r="67" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A67" s="4">
-        <v>287.0</v>
+        <v>287</v>
       </c>
       <c r="B67" s="4">
-        <v>189.0</v>
+        <v>189</v>
       </c>
       <c r="C67" s="4" t="s">
         <v>65</v>
       </c>
       <c r="D67" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E67" s="6">
         <v>44067.4375</v>
       </c>
       <c r="F67" s="3"/>
     </row>
-    <row r="68">
+    <row r="68" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A68" s="4">
-        <v>288.0</v>
+        <v>288</v>
       </c>
       <c r="B68" s="4">
-        <v>190.0</v>
+        <v>190</v>
       </c>
       <c r="C68" s="4" t="s">
         <v>66</v>
       </c>
       <c r="D68" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E68" s="6">
         <v>44067.375</v>
       </c>
       <c r="F68" s="3"/>
     </row>
-    <row r="69">
+    <row r="69" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A69" s="4">
-        <v>289.0</v>
+        <v>289</v>
       </c>
       <c r="B69" s="4">
-        <v>191.0</v>
+        <v>191</v>
       </c>
       <c r="C69" s="4" t="s">
         <v>67</v>
       </c>
       <c r="D69" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E69" s="6">
         <v>44066.75</v>
       </c>
       <c r="F69" s="3"/>
     </row>
-    <row r="70">
+    <row r="70" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A70" s="4">
-        <v>290.0</v>
+        <v>290</v>
       </c>
       <c r="B70" s="4">
-        <v>192.0</v>
+        <v>192</v>
       </c>
       <c r="C70" s="4" t="s">
         <v>68</v>
       </c>
       <c r="D70" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E70" s="6">
         <v>44066.833333333336</v>
       </c>
       <c r="F70" s="3"/>
     </row>
-    <row r="71">
+    <row r="71" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A71" s="4">
-        <v>291.0</v>
+        <v>291</v>
       </c>
       <c r="B71" s="4">
-        <v>193.0</v>
+        <v>193</v>
       </c>
       <c r="C71" s="4" t="s">
         <v>69</v>
       </c>
       <c r="D71" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E71" s="6">
         <v>44067.395833333336</v>
       </c>
       <c r="F71" s="3"/>
     </row>
-    <row r="72">
+    <row r="72" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A72" s="4">
-        <v>292.0</v>
+        <v>292</v>
       </c>
       <c r="B72" s="4">
-        <v>194.0</v>
+        <v>194</v>
       </c>
       <c r="C72" s="4" t="s">
         <v>70</v>
       </c>
       <c r="D72" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E72" s="6">
         <v>44067.15625</v>
       </c>
       <c r="F72" s="3"/>
     </row>
-    <row r="73">
+    <row r="73" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A73" s="4">
-        <v>293.0</v>
+        <v>293</v>
       </c>
       <c r="B73" s="4">
-        <v>195.0</v>
+        <v>195</v>
       </c>
       <c r="C73" s="4" t="s">
         <v>71</v>
       </c>
       <c r="D73" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E73" s="6">
         <v>44067.416666666664</v>
       </c>
       <c r="F73" s="3"/>
     </row>
-    <row r="74">
+    <row r="74" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A74" s="4">
-        <v>294.0</v>
+        <v>294</v>
       </c>
       <c r="B74" s="4">
-        <v>196.0</v>
+        <v>196</v>
       </c>
       <c r="C74" s="4" t="s">
         <v>72</v>
       </c>
       <c r="D74" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E74" s="6">
         <v>44067.4375</v>
       </c>
       <c r="F74" s="3"/>
     </row>
-    <row r="75">
+    <row r="75" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A75" s="4">
-        <v>295.0</v>
+        <v>295</v>
       </c>
       <c r="B75" s="4">
-        <v>197.0</v>
+        <v>197</v>
       </c>
       <c r="C75" s="4" t="s">
         <v>73</v>
       </c>
       <c r="D75" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E75" s="6">
         <v>44067.375</v>
       </c>
       <c r="F75" s="3"/>
     </row>
-    <row r="76">
+    <row r="76" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A76" s="4">
-        <v>296.0</v>
+        <v>296</v>
       </c>
       <c r="B76" s="4">
-        <v>198.0</v>
+        <v>198</v>
       </c>
       <c r="C76" s="4" t="s">
         <v>73</v>
       </c>
       <c r="D76" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E76" s="6">
         <v>44066.75</v>
       </c>
       <c r="F76" s="3"/>
     </row>
-    <row r="77">
+    <row r="77" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A77" s="4">
-        <v>297.0</v>
+        <v>297</v>
       </c>
       <c r="B77" s="4">
-        <v>199.0</v>
+        <v>199</v>
       </c>
       <c r="C77" s="4" t="s">
         <v>73</v>
       </c>
       <c r="D77" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E77" s="6">
         <v>44066.833333333336</v>
       </c>
       <c r="F77" s="3"/>
     </row>
-    <row r="78">
+    <row r="78" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A78" s="4">
-        <v>298.0</v>
+        <v>298</v>
       </c>
       <c r="B78" s="4">
-        <v>200.0</v>
+        <v>200</v>
       </c>
       <c r="C78" s="4" t="s">
         <v>74</v>
       </c>
       <c r="D78" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E78" s="6">
         <v>44067.395833333336</v>
       </c>
       <c r="F78" s="3"/>
     </row>
-    <row r="79">
+    <row r="79" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A79" s="4">
-        <v>299.0</v>
+        <v>299</v>
       </c>
       <c r="B79" s="4">
-        <v>201.0</v>
+        <v>201</v>
       </c>
       <c r="C79" s="4" t="s">
         <v>74</v>
       </c>
       <c r="D79" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E79" s="6">
         <v>44067.15625</v>
       </c>
       <c r="F79" s="3"/>
     </row>
-    <row r="80">
+    <row r="80" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A80" s="4">
-        <v>300.0</v>
+        <v>300</v>
       </c>
       <c r="B80" s="4">
-        <v>202.0</v>
+        <v>202</v>
       </c>
       <c r="C80" s="4" t="s">
         <v>75</v>
       </c>
       <c r="D80" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E80" s="6">
         <v>44067.416666666664</v>
       </c>
       <c r="F80" s="3"/>
     </row>
-    <row r="81">
+    <row r="81" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A81" s="4">
-        <v>301.0</v>
+        <v>301</v>
       </c>
       <c r="B81" s="4">
-        <v>203.0</v>
+        <v>203</v>
       </c>
       <c r="C81" s="4" t="s">
         <v>76</v>
       </c>
       <c r="D81" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E81" s="6">
         <v>44067.4375</v>
       </c>
       <c r="F81" s="3"/>
     </row>
-    <row r="82">
+    <row r="82" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A82" s="4">
-        <v>302.0</v>
+        <v>302</v>
       </c>
       <c r="B82" s="4">
-        <v>204.0</v>
+        <v>204</v>
       </c>
       <c r="C82" s="4" t="s">
         <v>77</v>
       </c>
       <c r="D82" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E82" s="6">
         <v>44067.375</v>
       </c>
       <c r="F82" s="3"/>
     </row>
-    <row r="83">
+    <row r="83" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A83" s="4">
-        <v>303.0</v>
+        <v>303</v>
       </c>
       <c r="B83" s="4">
-        <v>205.0</v>
+        <v>205</v>
       </c>
       <c r="C83" s="4" t="s">
         <v>78</v>
       </c>
       <c r="D83" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E83" s="6">
         <v>44066.75</v>
       </c>
       <c r="F83" s="3"/>
     </row>
-    <row r="84">
+    <row r="84" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A84" s="4">
-        <v>304.0</v>
+        <v>304</v>
       </c>
       <c r="B84" s="4">
-        <v>206.0</v>
+        <v>206</v>
       </c>
       <c r="C84" s="4" t="s">
         <v>79</v>
       </c>
       <c r="D84" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E84" s="6">
         <v>44066.833333333336</v>
       </c>
       <c r="F84" s="3"/>
     </row>
-    <row r="85">
+    <row r="85" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A85" s="4">
-        <v>305.0</v>
+        <v>305</v>
       </c>
       <c r="B85" s="4">
-        <v>207.0</v>
+        <v>207</v>
       </c>
       <c r="C85" s="4" t="s">
         <v>80</v>
       </c>
       <c r="D85" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E85" s="6">
         <v>44067.395833333336</v>
       </c>
       <c r="F85" s="3"/>
     </row>
-    <row r="86">
+    <row r="86" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A86" s="4">
-        <v>306.0</v>
+        <v>306</v>
       </c>
       <c r="B86" s="4">
-        <v>208.0</v>
+        <v>208</v>
       </c>
       <c r="C86" s="4" t="s">
         <v>81</v>
       </c>
       <c r="D86" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E86" s="6">
         <v>44067.15625</v>
       </c>
       <c r="F86" s="3"/>
     </row>
-    <row r="87">
+    <row r="87" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A87" s="4">
-        <v>307.0</v>
+        <v>307</v>
       </c>
       <c r="B87" s="4">
-        <v>209.0</v>
+        <v>209</v>
       </c>
       <c r="C87" s="4" t="s">
         <v>82</v>
       </c>
       <c r="D87" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E87" s="6">
         <v>44067.416666666664</v>
       </c>
       <c r="F87" s="3"/>
     </row>
-    <row r="88">
+    <row r="88" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A88" s="4">
-        <v>308.0</v>
+        <v>308</v>
       </c>
       <c r="B88" s="4">
-        <v>210.0</v>
+        <v>210</v>
       </c>
       <c r="C88" s="4" t="s">
         <v>83</v>
       </c>
       <c r="D88" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E88" s="6">
         <v>44067.4375</v>
       </c>
       <c r="F88" s="3"/>
     </row>
-    <row r="89">
+    <row r="89" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A89" s="4">
-        <v>309.0</v>
+        <v>309</v>
       </c>
       <c r="B89" s="4">
-        <v>211.0</v>
+        <v>211</v>
       </c>
       <c r="C89" s="4" t="s">
         <v>84</v>
       </c>
       <c r="D89" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E89" s="6">
         <v>44067.375</v>
       </c>
       <c r="F89" s="3"/>
     </row>
-    <row r="90">
+    <row r="90" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A90" s="4">
-        <v>310.0</v>
+        <v>310</v>
       </c>
       <c r="B90" s="4">
-        <v>212.0</v>
+        <v>212</v>
       </c>
       <c r="C90" s="4" t="s">
         <v>85</v>
       </c>
       <c r="D90" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E90" s="6">
         <v>44066.75</v>
       </c>
       <c r="F90" s="3"/>
     </row>
-    <row r="91">
+    <row r="91" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A91" s="4">
-        <v>311.0</v>
+        <v>311</v>
       </c>
       <c r="B91" s="4">
-        <v>213.0</v>
+        <v>213</v>
       </c>
       <c r="C91" s="4" t="s">
         <v>86</v>
       </c>
       <c r="D91" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E91" s="6">
         <v>44066.833333333336</v>
       </c>
       <c r="F91" s="3"/>
     </row>
-    <row r="92">
+    <row r="92" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A92" s="4">
-        <v>312.0</v>
+        <v>312</v>
       </c>
       <c r="B92" s="4">
-        <v>214.0</v>
+        <v>214</v>
       </c>
       <c r="C92" s="4" t="s">
         <v>87</v>
       </c>
       <c r="D92" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E92" s="6">
         <v>44067.395833333336</v>
       </c>
       <c r="F92" s="3"/>
     </row>
-    <row r="93">
+    <row r="93" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A93" s="4">
-        <v>313.0</v>
+        <v>313</v>
       </c>
       <c r="B93" s="4">
-        <v>215.0</v>
+        <v>215</v>
       </c>
       <c r="C93" s="4" t="s">
         <v>88</v>
       </c>
       <c r="D93" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E93" s="6">
         <v>44067.15625</v>
       </c>
       <c r="F93" s="3"/>
     </row>
-    <row r="94">
+    <row r="94" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A94" s="4">
-        <v>314.0</v>
+        <v>314</v>
       </c>
       <c r="B94" s="4">
-        <v>216.0</v>
+        <v>216</v>
       </c>
       <c r="C94" s="4" t="s">
         <v>89</v>
       </c>
       <c r="D94" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E94" s="6">
         <v>44067.416666666664</v>
       </c>
       <c r="F94" s="3"/>
     </row>
-    <row r="95">
+    <row r="95" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A95" s="4">
-        <v>315.0</v>
+        <v>315</v>
       </c>
       <c r="B95" s="4">
-        <v>217.0</v>
+        <v>217</v>
       </c>
       <c r="C95" s="4" t="s">
         <v>90</v>
       </c>
       <c r="D95" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E95" s="6">
         <v>44067.4375</v>
       </c>
       <c r="F95" s="3"/>
     </row>
-    <row r="96">
+    <row r="96" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A96" s="4">
-        <v>316.0</v>
+        <v>316</v>
       </c>
       <c r="B96" s="4">
-        <v>218.0</v>
+        <v>218</v>
       </c>
       <c r="C96" s="4" t="s">
         <v>91</v>
       </c>
       <c r="D96" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E96" s="6">
         <v>44067.375</v>
       </c>
       <c r="F96" s="3"/>
     </row>
-    <row r="97">
+    <row r="97" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A97" s="4">
-        <v>317.0</v>
+        <v>317</v>
       </c>
       <c r="B97" s="4">
-        <v>219.0</v>
+        <v>219</v>
       </c>
       <c r="C97" s="4" t="s">
         <v>92</v>
       </c>
       <c r="D97" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E97" s="6">
         <v>44066.75</v>
       </c>
       <c r="F97" s="3"/>
     </row>
-    <row r="98">
+    <row r="98" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A98" s="4">
-        <v>318.0</v>
+        <v>318</v>
       </c>
       <c r="B98" s="4">
-        <v>220.0</v>
+        <v>220</v>
       </c>
       <c r="C98" s="4" t="s">
         <v>93</v>
       </c>
       <c r="D98" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E98" s="6">
         <v>44066.833333333336</v>
       </c>
       <c r="F98" s="3"/>
     </row>
-    <row r="99">
+    <row r="99" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A99" s="4">
-        <v>319.0</v>
+        <v>319</v>
       </c>
       <c r="B99" s="4">
-        <v>221.0</v>
+        <v>221</v>
       </c>
       <c r="C99" s="4" t="s">
         <v>94</v>
       </c>
       <c r="D99" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E99" s="6">
         <v>44067.395833333336</v>
       </c>
       <c r="F99" s="3"/>
     </row>
-    <row r="100">
+    <row r="100" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A100" s="4">
-        <v>320.0</v>
+        <v>320</v>
       </c>
       <c r="B100" s="4">
-        <v>222.0</v>
+        <v>222</v>
       </c>
       <c r="C100" s="4" t="s">
         <v>95</v>
       </c>
       <c r="D100" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E100" s="6">
         <v>44067.15625</v>
       </c>
       <c r="F100" s="3"/>
     </row>
-    <row r="101">
+    <row r="101" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A101" s="4">
-        <v>321.0</v>
+        <v>321</v>
       </c>
       <c r="B101" s="4">
-        <v>223.0</v>
+        <v>223</v>
       </c>
       <c r="C101" s="4" t="s">
         <v>96</v>
       </c>
       <c r="D101" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E101" s="6">
         <v>44067.416666666664</v>
       </c>
       <c r="F101" s="3"/>
     </row>
-    <row r="102">
+    <row r="102" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A102" s="4">
-        <v>322.0</v>
+        <v>322</v>
       </c>
       <c r="B102" s="4">
-        <v>224.0</v>
+        <v>224</v>
       </c>
       <c r="C102" s="4" t="s">
         <v>97</v>
       </c>
       <c r="D102" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E102" s="6">
         <v>44067.4375</v>
       </c>
       <c r="F102" s="3"/>
     </row>
-    <row r="103">
+    <row r="103" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A103" s="4">
-        <v>323.0</v>
+        <v>323</v>
       </c>
       <c r="B103" s="4">
-        <v>225.0</v>
+        <v>225</v>
       </c>
       <c r="C103" s="4" t="s">
         <v>98</v>
       </c>
       <c r="D103" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E103" s="6">
         <v>44067.375</v>
       </c>
       <c r="F103" s="3"/>
     </row>
-    <row r="104">
+    <row r="104" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A104" s="4">
-        <v>324.0</v>
+        <v>324</v>
       </c>
       <c r="B104" s="4">
-        <v>226.0</v>
+        <v>226</v>
       </c>
       <c r="C104" s="4" t="s">
         <v>99</v>
       </c>
       <c r="D104" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E104" s="6">
         <v>44066.75</v>
       </c>
       <c r="F104" s="3"/>
     </row>
-    <row r="105">
+    <row r="105" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A105" s="4">
-        <v>325.0</v>
+        <v>325</v>
       </c>
       <c r="B105" s="4">
-        <v>227.0</v>
+        <v>227</v>
       </c>
       <c r="C105" s="4" t="s">
         <v>100</v>
       </c>
       <c r="D105" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E105" s="6">
         <v>44066.833333333336</v>
       </c>
       <c r="F105" s="3"/>
     </row>
-    <row r="106">
+    <row r="106" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A106" s="4">
-        <v>326.0</v>
+        <v>326</v>
       </c>
       <c r="B106" s="4">
-        <v>228.0</v>
+        <v>228</v>
       </c>
       <c r="C106" s="4" t="s">
         <v>101</v>
       </c>
       <c r="D106" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E106" s="6">
         <v>44067.395833333336</v>
       </c>
       <c r="F106" s="3"/>
     </row>
-    <row r="107">
+    <row r="107" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A107" s="4">
-        <v>327.0</v>
+        <v>327</v>
       </c>
       <c r="B107" s="4">
-        <v>229.0</v>
+        <v>229</v>
       </c>
       <c r="C107" s="4" t="s">
         <v>102</v>
       </c>
       <c r="D107" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E107" s="6">
         <v>44067.15625</v>
       </c>
       <c r="F107" s="3"/>
     </row>
-    <row r="108">
+    <row r="108" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A108" s="4">
-        <v>328.0</v>
+        <v>328</v>
       </c>
       <c r="B108" s="4">
-        <v>230.0</v>
+        <v>230</v>
       </c>
       <c r="C108" s="4" t="s">
         <v>102</v>
       </c>
       <c r="D108" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E108" s="6">
         <v>44067.416666666664</v>
       </c>
       <c r="F108" s="3"/>
     </row>
-    <row r="109">
+    <row r="109" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A109" s="4">
-        <v>329.0</v>
+        <v>329</v>
       </c>
       <c r="B109" s="4">
-        <v>231.0</v>
+        <v>231</v>
       </c>
       <c r="C109" s="4" t="s">
         <v>103</v>
       </c>
       <c r="D109" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E109" s="6">
         <v>44067.4375</v>
       </c>
       <c r="F109" s="3"/>
     </row>
-    <row r="110">
+    <row r="110" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A110" s="4">
-        <v>330.0</v>
+        <v>330</v>
       </c>
       <c r="B110" s="4">
-        <v>232.0</v>
+        <v>232</v>
       </c>
       <c r="C110" s="4" t="s">
         <v>104</v>
       </c>
       <c r="D110" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E110" s="6">
         <v>44067.375</v>
       </c>
       <c r="F110" s="3"/>
     </row>
-    <row r="111">
+    <row r="111" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A111" s="4">
-        <v>331.0</v>
+        <v>331</v>
       </c>
       <c r="B111" s="4">
-        <v>233.0</v>
+        <v>233</v>
       </c>
       <c r="C111" s="4" t="s">
         <v>105</v>
       </c>
       <c r="D111" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E111" s="6">
         <v>44066.75</v>
       </c>
       <c r="F111" s="3"/>
     </row>
-    <row r="112">
+    <row r="112" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A112" s="4">
-        <v>332.0</v>
+        <v>332</v>
       </c>
       <c r="B112" s="4">
-        <v>234.0</v>
+        <v>234</v>
       </c>
       <c r="C112" s="4" t="s">
         <v>106</v>
       </c>
       <c r="D112" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E112" s="6">
         <v>44066.833333333336</v>
       </c>
       <c r="F112" s="3"/>
     </row>
-    <row r="113">
+    <row r="113" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A113" s="4">
-        <v>333.0</v>
+        <v>333</v>
       </c>
       <c r="B113" s="4">
-        <v>235.0</v>
+        <v>235</v>
       </c>
       <c r="C113" s="4" t="s">
         <v>107</v>
       </c>
       <c r="D113" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E113" s="6">
         <v>44067.395833333336</v>
       </c>
       <c r="F113" s="3"/>
     </row>
-    <row r="114">
+    <row r="114" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A114" s="4">
-        <v>334.0</v>
+        <v>334</v>
       </c>
       <c r="B114" s="4">
-        <v>236.0</v>
+        <v>236</v>
       </c>
       <c r="C114" s="4" t="s">
         <v>108</v>
       </c>
       <c r="D114" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E114" s="6">
         <v>44067.15625</v>
       </c>
       <c r="F114" s="3"/>
     </row>
-    <row r="115">
+    <row r="115" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A115" s="4">
-        <v>335.0</v>
+        <v>335</v>
       </c>
       <c r="B115" s="4">
-        <v>237.0</v>
+        <v>237</v>
       </c>
       <c r="C115" s="4" t="s">
         <v>109</v>
       </c>
       <c r="D115" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E115" s="6">
         <v>44067.416666666664</v>
       </c>
       <c r="F115" s="3"/>
     </row>
-    <row r="116">
+    <row r="116" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A116" s="4">
-        <v>336.0</v>
+        <v>336</v>
       </c>
       <c r="B116" s="4">
-        <v>238.0</v>
+        <v>238</v>
       </c>
       <c r="C116" s="4" t="s">
         <v>110</v>
       </c>
       <c r="D116" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E116" s="6">
         <v>44067.4375</v>
       </c>
       <c r="F116" s="3"/>
     </row>
-    <row r="117">
+    <row r="117" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A117" s="4">
-        <v>337.0</v>
+        <v>337</v>
       </c>
       <c r="B117" s="4">
-        <v>239.0</v>
+        <v>239</v>
       </c>
       <c r="C117" s="4" t="s">
         <v>111</v>
       </c>
       <c r="D117" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E117" s="6">
         <v>44067.375</v>
       </c>
       <c r="F117" s="3"/>
     </row>
-    <row r="118">
+    <row r="118" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A118" s="4">
-        <v>338.0</v>
+        <v>338</v>
       </c>
       <c r="B118" s="4">
-        <v>240.0</v>
+        <v>240</v>
       </c>
       <c r="C118" s="4" t="s">
         <v>112</v>
       </c>
       <c r="D118" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E118" s="6">
         <v>44066.75</v>
       </c>
       <c r="F118" s="3"/>
     </row>
-    <row r="119">
+    <row r="119" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A119" s="4">
-        <v>339.0</v>
+        <v>339</v>
       </c>
       <c r="B119" s="4">
-        <v>241.0</v>
+        <v>241</v>
       </c>
       <c r="C119" s="4" t="s">
         <v>113</v>
       </c>
       <c r="D119" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E119" s="6">
         <v>44066.833333333336</v>
       </c>
       <c r="F119" s="3"/>
     </row>
-    <row r="120">
+    <row r="120" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A120" s="4">
-        <v>340.0</v>
+        <v>340</v>
       </c>
       <c r="B120" s="4">
-        <v>242.0</v>
+        <v>242</v>
       </c>
       <c r="C120" s="4" t="s">
         <v>114</v>
       </c>
       <c r="D120" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E120" s="6">
         <v>44067.395833333336</v>
       </c>
       <c r="F120" s="3"/>
     </row>
-    <row r="121">
+    <row r="121" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A121" s="4">
-        <v>341.0</v>
+        <v>341</v>
       </c>
       <c r="B121" s="4">
-        <v>243.0</v>
+        <v>243</v>
       </c>
       <c r="C121" s="4" t="s">
         <v>115</v>
       </c>
       <c r="D121" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E121" s="6">
         <v>44067.15625</v>
       </c>
       <c r="F121" s="3"/>
     </row>
-    <row r="122">
+    <row r="122" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A122" s="4">
-        <v>342.0</v>
+        <v>342</v>
       </c>
       <c r="B122" s="4">
-        <v>244.0</v>
+        <v>244</v>
       </c>
       <c r="C122" s="4" t="s">
         <v>115</v>
       </c>
       <c r="D122" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E122" s="6">
         <v>44067.416666666664</v>
       </c>
       <c r="F122" s="3"/>
     </row>
-    <row r="123">
+    <row r="123" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A123" s="4">
-        <v>343.0</v>
+        <v>343</v>
       </c>
       <c r="B123" s="4">
-        <v>245.0</v>
+        <v>245</v>
       </c>
       <c r="C123" s="4" t="s">
         <v>116</v>
       </c>
       <c r="D123" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E123" s="6">
         <v>44067.4375</v>
       </c>
       <c r="F123" s="3"/>
     </row>
-    <row r="124">
+    <row r="124" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A124" s="4">
-        <v>344.0</v>
+        <v>344</v>
       </c>
       <c r="B124" s="4">
-        <v>246.0</v>
+        <v>246</v>
       </c>
       <c r="C124" s="4" t="s">
         <v>117</v>
       </c>
       <c r="D124" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E124" s="6">
         <v>44067.375</v>
       </c>
       <c r="F124" s="3"/>
     </row>
-    <row r="125">
+    <row r="125" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A125" s="4">
-        <v>345.0</v>
+        <v>345</v>
       </c>
       <c r="B125" s="4">
-        <v>247.0</v>
+        <v>247</v>
       </c>
       <c r="C125" s="4" t="s">
         <v>118</v>
       </c>
       <c r="D125" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E125" s="6">
         <v>44066.75</v>
       </c>
       <c r="F125" s="3"/>
     </row>
-    <row r="126">
+    <row r="126" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A126" s="4">
-        <v>346.0</v>
+        <v>346</v>
       </c>
       <c r="B126" s="4">
-        <v>248.0</v>
+        <v>248</v>
       </c>
       <c r="C126" s="4" t="s">
         <v>119</v>
       </c>
       <c r="D126" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E126" s="6">
         <v>44066.833333333336</v>
       </c>
       <c r="F126" s="3"/>
     </row>
-    <row r="127">
+    <row r="127" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A127" s="4">
-        <v>347.0</v>
+        <v>347</v>
       </c>
       <c r="B127" s="4">
-        <v>249.0</v>
+        <v>249</v>
       </c>
       <c r="C127" s="4" t="s">
         <v>120</v>
       </c>
       <c r="D127" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E127" s="6">
         <v>44067.395833333336</v>
       </c>
       <c r="F127" s="3"/>
     </row>
-    <row r="128">
+    <row r="128" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A128" s="4">
-        <v>348.0</v>
+        <v>348</v>
       </c>
       <c r="B128" s="4">
-        <v>250.0</v>
+        <v>250</v>
       </c>
       <c r="C128" s="4" t="s">
         <v>121</v>
       </c>
       <c r="D128" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E128" s="6">
         <v>44067.15625</v>
       </c>
       <c r="F128" s="3"/>
     </row>
-    <row r="129">
+    <row r="129" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A129" s="4">
-        <v>349.0</v>
+        <v>349</v>
       </c>
       <c r="B129" s="4">
-        <v>251.0</v>
+        <v>251</v>
       </c>
       <c r="C129" s="4" t="s">
         <v>122</v>
       </c>
       <c r="D129" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E129" s="6">
         <v>44067.416666666664</v>
       </c>
       <c r="F129" s="3"/>
     </row>
-    <row r="130">
+    <row r="130" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A130" s="4">
-        <v>350.0</v>
+        <v>350</v>
       </c>
       <c r="B130" s="4">
-        <v>252.0</v>
+        <v>252</v>
       </c>
       <c r="C130" s="4" t="s">
         <v>123</v>
       </c>
       <c r="D130" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E130" s="6">
         <v>44067.4375</v>
       </c>
       <c r="F130" s="3"/>
     </row>
-    <row r="131">
+    <row r="131" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A131" s="4">
-        <v>351.0</v>
+        <v>351</v>
       </c>
       <c r="B131" s="4">
-        <v>253.0</v>
+        <v>253</v>
       </c>
       <c r="C131" s="4" t="s">
         <v>124</v>
       </c>
       <c r="D131" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E131" s="6">
         <v>44067.375</v>
       </c>
       <c r="F131" s="3"/>
     </row>
-    <row r="132">
+    <row r="132" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A132" s="4">
-        <v>352.0</v>
+        <v>352</v>
       </c>
       <c r="B132" s="4">
-        <v>254.0</v>
+        <v>254</v>
       </c>
       <c r="C132" s="4" t="s">
         <v>125</v>
       </c>
       <c r="D132" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E132" s="6">
         <v>44066.75</v>
       </c>
       <c r="F132" s="3"/>
     </row>
-    <row r="133">
+    <row r="133" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A133" s="4">
-        <v>353.0</v>
+        <v>353</v>
       </c>
       <c r="B133" s="4">
-        <v>255.0</v>
+        <v>255</v>
       </c>
       <c r="C133" s="4" t="s">
         <v>126</v>
       </c>
       <c r="D133" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E133" s="6">
         <v>44066.833333333336</v>
       </c>
       <c r="F133" s="3"/>
     </row>
-    <row r="134">
+    <row r="134" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A134" s="4">
-        <v>354.0</v>
+        <v>354</v>
       </c>
       <c r="B134" s="4">
-        <v>256.0</v>
+        <v>256</v>
       </c>
       <c r="C134" s="4" t="s">
         <v>127</v>
       </c>
       <c r="D134" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E134" s="6">
         <v>44067.395833333336</v>
       </c>
       <c r="F134" s="3"/>
     </row>
-    <row r="135">
+    <row r="135" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A135" s="4">
-        <v>355.0</v>
+        <v>355</v>
       </c>
       <c r="B135" s="4">
-        <v>257.0</v>
+        <v>257</v>
       </c>
       <c r="C135" s="4" t="s">
         <v>128</v>
       </c>
       <c r="D135" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E135" s="6">
         <v>44067.15625</v>
       </c>
       <c r="F135" s="3"/>
     </row>
-    <row r="136">
+    <row r="136" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A136" s="4">
-        <v>356.0</v>
+        <v>356</v>
       </c>
       <c r="B136" s="4">
-        <v>258.0</v>
+        <v>258</v>
       </c>
       <c r="C136" s="4" t="s">
         <v>129</v>
       </c>
       <c r="D136" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E136" s="6">
         <v>44067.416666666664</v>
       </c>
       <c r="F136" s="3"/>
     </row>
-    <row r="137">
+    <row r="137" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A137" s="4">
-        <v>357.0</v>
+        <v>357</v>
       </c>
       <c r="B137" s="4">
-        <v>259.0</v>
+        <v>259</v>
       </c>
       <c r="C137" s="4" t="s">
         <v>130</v>
       </c>
       <c r="D137" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E137" s="6">
         <v>44067.4375</v>
       </c>
       <c r="F137" s="3"/>
     </row>
-    <row r="138">
+    <row r="138" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A138" s="4">
-        <v>358.0</v>
+        <v>358</v>
       </c>
       <c r="B138" s="4">
-        <v>260.0</v>
+        <v>260</v>
       </c>
       <c r="C138" s="4" t="s">
         <v>131</v>
       </c>
       <c r="D138" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E138" s="6">
         <v>44067.375</v>
       </c>
       <c r="F138" s="3"/>
     </row>
-    <row r="139">
+    <row r="139" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A139" s="4">
-        <v>359.0</v>
+        <v>359</v>
       </c>
       <c r="B139" s="4">
-        <v>261.0</v>
+        <v>261</v>
       </c>
       <c r="C139" s="4" t="s">
         <v>132</v>
       </c>
       <c r="D139" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E139" s="6">
         <v>44066.75</v>
       </c>
       <c r="F139" s="3"/>
     </row>
-    <row r="140">
+    <row r="140" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A140" s="4">
-        <v>360.0</v>
+        <v>360</v>
       </c>
       <c r="B140" s="4">
-        <v>262.0</v>
+        <v>262</v>
       </c>
       <c r="C140" s="4" t="s">
         <v>133</v>
       </c>
       <c r="D140" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E140" s="6">
         <v>44066.833333333336</v>
       </c>
       <c r="F140" s="3"/>
     </row>
-    <row r="141">
+    <row r="141" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A141" s="4">
-        <v>361.0</v>
+        <v>361</v>
       </c>
       <c r="B141" s="4">
-        <v>263.0</v>
+        <v>263</v>
       </c>
       <c r="C141" s="4" t="s">
         <v>134</v>
       </c>
       <c r="D141" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E141" s="6">
         <v>44067.395833333336</v>
       </c>
       <c r="F141" s="3"/>
     </row>
-    <row r="142">
+    <row r="142" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A142" s="4">
-        <v>362.0</v>
+        <v>362</v>
       </c>
       <c r="B142" s="4">
-        <v>264.0</v>
+        <v>264</v>
       </c>
       <c r="C142" s="4" t="s">
         <v>135</v>
       </c>
       <c r="D142" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E142" s="6">
         <v>44067.15625</v>
       </c>
       <c r="F142" s="3"/>
     </row>
-    <row r="143">
+    <row r="143" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A143" s="4">
-        <v>363.0</v>
+        <v>363</v>
       </c>
       <c r="B143" s="4">
-        <v>265.0</v>
+        <v>265</v>
       </c>
       <c r="C143" s="4" t="s">
         <v>136</v>
       </c>
       <c r="D143" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E143" s="6">
         <v>44067.416666666664</v>
       </c>
       <c r="F143" s="3"/>
     </row>
-    <row r="144">
+    <row r="144" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A144" s="4">
-        <v>364.0</v>
+        <v>364</v>
       </c>
       <c r="B144" s="4">
-        <v>266.0</v>
+        <v>266</v>
       </c>
       <c r="C144" s="4" t="s">
         <v>137</v>
       </c>
       <c r="D144" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E144" s="6">
         <v>44067.4375</v>
       </c>
       <c r="F144" s="3"/>
     </row>
-    <row r="145">
+    <row r="145" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A145" s="4">
-        <v>365.0</v>
+        <v>365</v>
       </c>
       <c r="B145" s="4">
-        <v>267.0</v>
+        <v>267</v>
       </c>
       <c r="C145" s="4" t="s">
         <v>138</v>
       </c>
       <c r="D145" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E145" s="6">
         <v>44067.375</v>
       </c>
       <c r="F145" s="3"/>
     </row>
-    <row r="146">
+    <row r="146" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A146" s="4">
-        <v>366.0</v>
+        <v>366</v>
       </c>
       <c r="B146" s="4">
-        <v>268.0</v>
+        <v>268</v>
       </c>
       <c r="C146" s="4" t="s">
         <v>139</v>
       </c>
       <c r="D146" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E146" s="6">
         <v>44066.75</v>
       </c>
       <c r="F146" s="3"/>
     </row>
-    <row r="147">
+    <row r="147" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A147" s="4">
-        <v>367.0</v>
+        <v>367</v>
       </c>
       <c r="B147" s="4">
-        <v>269.0</v>
+        <v>269</v>
       </c>
       <c r="C147" s="4" t="s">
         <v>140</v>
       </c>
       <c r="D147" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E147" s="6">
         <v>44066.833333333336</v>
       </c>
       <c r="F147" s="3"/>
     </row>
-    <row r="148">
+    <row r="148" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A148" s="4">
-        <v>368.0</v>
+        <v>368</v>
       </c>
       <c r="B148" s="4">
-        <v>270.0</v>
+        <v>270</v>
       </c>
       <c r="C148" s="4" t="s">
         <v>141</v>
       </c>
       <c r="D148" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E148" s="6">
         <v>44067.395833333336</v>
       </c>
       <c r="F148" s="3"/>
     </row>
-    <row r="149">
+    <row r="149" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A149" s="4">
-        <v>369.0</v>
+        <v>369</v>
       </c>
       <c r="B149" s="4">
-        <v>271.0</v>
+        <v>271</v>
       </c>
       <c r="C149" s="4" t="s">
         <v>142</v>
       </c>
       <c r="D149" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E149" s="6">
         <v>44067.15625</v>
       </c>
       <c r="F149" s="3"/>
     </row>
-    <row r="150">
+    <row r="150" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A150" s="4">
-        <v>370.0</v>
+        <v>370</v>
       </c>
       <c r="B150" s="4">
-        <v>272.0</v>
+        <v>272</v>
       </c>
       <c r="C150" s="4" t="s">
         <v>143</v>
       </c>
       <c r="D150" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E150" s="6">
         <v>44067.416666666664</v>
       </c>
       <c r="F150" s="3"/>
     </row>
-    <row r="151">
+    <row r="151" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A151" s="4">
-        <v>371.0</v>
+        <v>371</v>
       </c>
       <c r="B151" s="4">
-        <v>273.0</v>
+        <v>273</v>
       </c>
       <c r="C151" s="4" t="s">
         <v>144</v>
       </c>
       <c r="D151" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E151" s="6">
         <v>44067.4375</v>
       </c>
       <c r="F151" s="3"/>
     </row>
-    <row r="152">
+    <row r="152" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A152" s="4">
-        <v>372.0</v>
+        <v>372</v>
       </c>
       <c r="B152" s="4">
-        <v>274.0</v>
+        <v>274</v>
       </c>
       <c r="C152" s="4" t="s">
         <v>145</v>
       </c>
       <c r="D152" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E152" s="6">
         <v>44067.375</v>
       </c>
       <c r="F152" s="3"/>
     </row>
-    <row r="153">
+    <row r="153" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A153" s="4">
-        <v>373.0</v>
+        <v>373</v>
       </c>
       <c r="B153" s="4">
-        <v>275.0</v>
+        <v>275</v>
       </c>
       <c r="C153" s="4" t="s">
         <v>146</v>
       </c>
       <c r="D153" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E153" s="6">
         <v>44066.75</v>
       </c>
       <c r="F153" s="3"/>
     </row>
-    <row r="154">
+    <row r="154" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A154" s="4">
-        <v>374.0</v>
+        <v>374</v>
       </c>
       <c r="B154" s="4">
-        <v>276.0</v>
+        <v>276</v>
       </c>
       <c r="C154" s="4" t="s">
         <v>147</v>
       </c>
       <c r="D154" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E154" s="6">
         <v>44066.833333333336</v>
       </c>
       <c r="F154" s="3"/>
     </row>
-    <row r="155">
+    <row r="155" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A155" s="4">
-        <v>375.0</v>
+        <v>375</v>
       </c>
       <c r="B155" s="4">
-        <v>277.0</v>
+        <v>277</v>
       </c>
       <c r="C155" s="4" t="s">
         <v>147</v>
       </c>
       <c r="D155" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E155" s="6">
         <v>44067.395833333336</v>
       </c>
       <c r="F155" s="3"/>
     </row>
-    <row r="156">
+    <row r="156" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A156" s="4">
-        <v>376.0</v>
+        <v>376</v>
       </c>
       <c r="B156" s="4">
-        <v>278.0</v>
+        <v>278</v>
       </c>
       <c r="C156" s="4" t="s">
         <v>148</v>
       </c>
       <c r="D156" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E156" s="6">
         <v>44067.15625</v>
       </c>
       <c r="F156" s="3"/>
     </row>
-    <row r="157">
+    <row r="157" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A157" s="4">
-        <v>377.0</v>
+        <v>377</v>
       </c>
       <c r="B157" s="4">
-        <v>279.0</v>
+        <v>279</v>
       </c>
       <c r="C157" s="4" t="s">
         <v>149</v>
       </c>
       <c r="D157" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E157" s="6">
         <v>44067.416666666664</v>
       </c>
       <c r="F157" s="3"/>
     </row>
-    <row r="158">
+    <row r="158" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A158" s="4">
-        <v>378.0</v>
+        <v>378</v>
       </c>
       <c r="B158" s="4">
-        <v>280.0</v>
+        <v>280</v>
       </c>
       <c r="C158" s="4" t="s">
         <v>150</v>
       </c>
       <c r="D158" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E158" s="6">
         <v>44067.4375</v>
       </c>
       <c r="F158" s="3"/>
     </row>
-    <row r="159">
+    <row r="159" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A159" s="4">
-        <v>379.0</v>
+        <v>379</v>
       </c>
       <c r="B159" s="4">
-        <v>281.0</v>
+        <v>281</v>
       </c>
       <c r="C159" s="4" t="s">
         <v>151</v>
       </c>
       <c r="D159" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E159" s="6">
         <v>44067.375</v>
       </c>
       <c r="F159" s="3"/>
     </row>
-    <row r="160">
+    <row r="160" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A160" s="4">
-        <v>380.0</v>
+        <v>380</v>
       </c>
       <c r="B160" s="4">
-        <v>282.0</v>
+        <v>282</v>
       </c>
       <c r="C160" s="4" t="s">
         <v>152</v>
       </c>
       <c r="D160" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E160" s="6">
         <v>44066.75</v>
       </c>
       <c r="F160" s="3"/>
     </row>
-    <row r="161">
+    <row r="161" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A161" s="4">
-        <v>381.0</v>
+        <v>381</v>
       </c>
       <c r="B161" s="4">
-        <v>283.0</v>
+        <v>283</v>
       </c>
       <c r="C161" s="4" t="s">
         <v>153</v>
       </c>
       <c r="D161" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E161" s="6">
         <v>44066.833333333336</v>
       </c>
       <c r="F161" s="3"/>
     </row>
-    <row r="162">
+    <row r="162" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A162" s="4">
-        <v>382.0</v>
+        <v>382</v>
       </c>
       <c r="B162" s="4">
-        <v>284.0</v>
+        <v>284</v>
       </c>
       <c r="C162" s="4" t="s">
         <v>154</v>
       </c>
       <c r="D162" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E162" s="6">
         <v>44067.395833333336</v>
       </c>
       <c r="F162" s="3"/>
     </row>
-    <row r="163">
+    <row r="163" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A163" s="4">
-        <v>383.0</v>
+        <v>383</v>
       </c>
       <c r="B163" s="4">
-        <v>285.0</v>
+        <v>285</v>
       </c>
       <c r="C163" s="4" t="s">
         <v>155</v>
       </c>
       <c r="D163" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E163" s="6">
         <v>44067.15625</v>
       </c>
       <c r="F163" s="3"/>
     </row>
-    <row r="164">
+    <row r="164" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A164" s="4">
-        <v>384.0</v>
+        <v>384</v>
       </c>
       <c r="B164" s="4">
-        <v>286.0</v>
+        <v>286</v>
       </c>
       <c r="C164" s="4" t="s">
         <v>156</v>
       </c>
       <c r="D164" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E164" s="6">
         <v>44067.416666666664</v>
       </c>
       <c r="F164" s="3"/>
     </row>
-    <row r="165">
+    <row r="165" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A165" s="4">
-        <v>385.0</v>
+        <v>385</v>
       </c>
       <c r="B165" s="4">
-        <v>287.0</v>
+        <v>287</v>
       </c>
       <c r="C165" s="4" t="s">
         <v>157</v>
       </c>
       <c r="D165" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E165" s="6">
         <v>44067.4375</v>
       </c>
       <c r="F165" s="3"/>
     </row>
-    <row r="166">
+    <row r="166" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A166" s="4">
-        <v>386.0</v>
+        <v>386</v>
       </c>
       <c r="B166" s="4">
-        <v>288.0</v>
+        <v>288</v>
       </c>
       <c r="C166" s="4" t="s">
         <v>158</v>
       </c>
       <c r="D166" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E166" s="6">
         <v>44067.375</v>
       </c>
       <c r="F166" s="3"/>
     </row>
-    <row r="167">
+    <row r="167" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A167" s="4">
-        <v>387.0</v>
+        <v>387</v>
       </c>
       <c r="B167" s="4">
-        <v>289.0</v>
+        <v>289</v>
       </c>
       <c r="C167" s="4" t="s">
         <v>158</v>
       </c>
       <c r="D167" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E167" s="6">
         <v>44066.75</v>
       </c>
       <c r="F167" s="3"/>
     </row>
-    <row r="168">
+    <row r="168" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A168" s="4">
-        <v>388.0</v>
+        <v>388</v>
       </c>
       <c r="B168" s="4">
-        <v>290.0</v>
+        <v>290</v>
       </c>
       <c r="C168" s="4" t="s">
         <v>159</v>
       </c>
       <c r="D168" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E168" s="6">
         <v>44066.833333333336</v>
       </c>
       <c r="F168" s="3"/>
     </row>
-    <row r="169">
+    <row r="169" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A169" s="4">
-        <v>389.0</v>
+        <v>389</v>
       </c>
       <c r="B169" s="4">
-        <v>291.0</v>
+        <v>291</v>
       </c>
       <c r="C169" s="4" t="s">
         <v>160</v>
       </c>
       <c r="D169" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E169" s="6">
         <v>44067.395833333336</v>
       </c>
       <c r="F169" s="3"/>
     </row>
-    <row r="170">
+    <row r="170" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A170" s="4">
-        <v>390.0</v>
+        <v>390</v>
       </c>
       <c r="B170" s="4">
-        <v>292.0</v>
+        <v>292</v>
       </c>
       <c r="C170" s="4" t="s">
         <v>161</v>
       </c>
       <c r="D170" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E170" s="6">
         <v>44067.15625</v>
       </c>
       <c r="F170" s="3"/>
     </row>
-    <row r="171">
+    <row r="171" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A171" s="4">
-        <v>391.0</v>
+        <v>391</v>
       </c>
       <c r="B171" s="4">
-        <v>293.0</v>
+        <v>293</v>
       </c>
       <c r="C171" s="4" t="s">
         <v>162</v>
       </c>
       <c r="D171" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E171" s="6">
         <v>44067.416666666664</v>
       </c>
       <c r="F171" s="3"/>
     </row>
-    <row r="172">
+    <row r="172" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A172" s="4">
-        <v>392.0</v>
+        <v>392</v>
       </c>
       <c r="B172" s="4">
-        <v>294.0</v>
+        <v>294</v>
       </c>
       <c r="C172" s="4" t="s">
         <v>163</v>
       </c>
       <c r="D172" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E172" s="6">
         <v>44067.4375</v>
       </c>
       <c r="F172" s="3"/>
     </row>
-    <row r="173">
+    <row r="173" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A173" s="4">
-        <v>393.0</v>
+        <v>393</v>
       </c>
       <c r="B173" s="4">
-        <v>295.0</v>
+        <v>295</v>
       </c>
       <c r="C173" s="4" t="s">
         <v>164</v>
       </c>
       <c r="D173" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E173" s="6">
         <v>44067.375</v>
       </c>
       <c r="F173" s="3"/>
     </row>
-    <row r="174">
+    <row r="174" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A174" s="4">
-        <v>394.0</v>
+        <v>394</v>
       </c>
       <c r="B174" s="4">
-        <v>296.0</v>
+        <v>296</v>
       </c>
       <c r="C174" s="4" t="s">
         <v>165</v>
       </c>
       <c r="D174" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E174" s="6">
         <v>44066.75</v>
       </c>
       <c r="F174" s="3"/>
     </row>
-    <row r="175">
+    <row r="175" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A175" s="4">
-        <v>395.0</v>
+        <v>395</v>
       </c>
       <c r="B175" s="4">
-        <v>297.0</v>
+        <v>297</v>
       </c>
       <c r="C175" s="4" t="s">
         <v>166</v>
       </c>
       <c r="D175" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E175" s="6">
         <v>44066.833333333336</v>
       </c>
       <c r="F175" s="3"/>
     </row>
-    <row r="176">
+    <row r="176" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A176" s="4">
-        <v>396.0</v>
+        <v>396</v>
       </c>
       <c r="B176" s="4">
-        <v>298.0</v>
+        <v>298</v>
       </c>
       <c r="C176" s="4" t="s">
         <v>167</v>
       </c>
       <c r="D176" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E176" s="6">
         <v>44067.395833333336</v>
       </c>
       <c r="F176" s="3"/>
     </row>
-    <row r="177">
+    <row r="177" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A177" s="4">
-        <v>397.0</v>
+        <v>397</v>
       </c>
       <c r="B177" s="4">
-        <v>299.0</v>
+        <v>299</v>
       </c>
       <c r="C177" s="4" t="s">
         <v>168</v>
       </c>
       <c r="D177" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E177" s="6">
         <v>44066.833333333336</v>
       </c>
       <c r="F177" s="3"/>
     </row>
-    <row r="178">
+    <row r="178" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A178" s="4">
-        <v>398.0</v>
+        <v>398</v>
       </c>
       <c r="B178" s="4">
-        <v>300.0</v>
+        <v>300</v>
       </c>
       <c r="C178" s="4" t="s">
         <v>169</v>
       </c>
       <c r="D178" s="5">
-        <v>43975.0</v>
+        <v>43975</v>
       </c>
       <c r="E178" s="6">
         <v>44067.395833333336</v>
@@ -4012,6 +4033,6 @@
       <c r="F178" s="3"/>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>